<commit_message>
Aggiunto Doc Riuso Codice
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFA1E5-1DF9-4534-ABAD-984F4AF92164}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5CCC7B-F04C-4A5A-8867-6CC35D67847D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="17">
   <si>
     <t>LucaP</t>
   </si>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E1:I27"/>
+  <dimension ref="E1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,6 +888,23 @@
         <v>60</v>
       </c>
     </row>
+    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1">
+        <v>43525</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Inseriti form nel manuale
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF2ABAB-E00D-46AE-AC32-54A9B73D2300}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B65D8B8-1E93-4770-A735-FC7DA3C09553}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,22 @@
     <definedName name="Progetto">Foglio1!$B:$B</definedName>
     <definedName name="Tempo">Foglio1!$G:$G</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>LucaP</t>
   </si>
@@ -87,6 +92,9 @@
   </si>
   <si>
     <t>Full Calendar</t>
+  </si>
+  <si>
+    <t>Totale:</t>
   </si>
 </sst>
 </file>
@@ -422,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E1:I33"/>
+  <dimension ref="E1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +1002,32 @@
         <v>60</v>
       </c>
     </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>43546</v>
+      </c>
+      <c r="I34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <f>SUBTOTAL(109,I2:I35)</f>
+        <v>2040</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Homepage, E-R, tempi, db
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaP.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2CF9C5-5AE2-49EB-AE9F-0E62B758B1BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
     <definedName name="Progetto">Foglio1!$B:$B</definedName>
     <definedName name="Tempo">Foglio1!$G:$G</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
   <si>
     <t>LucaP</t>
   </si>
@@ -97,12 +98,15 @@
   </si>
   <si>
     <t>E-R</t>
+  </si>
+  <si>
+    <t>Db, E-R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,17 +157,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="E1:I1048576" totalsRowShown="0">
-  <autoFilter ref="E1:I1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="E1:I1048576" totalsRowShown="0">
+  <autoFilter ref="E1:I1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="E2:I15">
     <sortCondition ref="H1:H1048576"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="3" name="Persona"/>
-    <tableColumn id="4" name="Progetto"/>
-    <tableColumn id="1" name="Attività"/>
-    <tableColumn id="2" name="Data"/>
-    <tableColumn id="5" name="Tempo (min)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Persona"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progetto"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Attività"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tempo (min)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,11 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,13 +1093,30 @@
         <v>30</v>
       </c>
     </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="1">
+        <v>43558</v>
+      </c>
+      <c r="I39">
+        <v>50</v>
+      </c>
+    </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>20</v>
       </c>
       <c r="I41">
         <f>SUBTOTAL(109,I2:I40)</f>
-        <v>2310</v>
+        <v>2360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>